<commit_message>
Ya se generan facturas
</commit_message>
<xml_diff>
--- a/public/excel/facturas.xlsx
+++ b/public/excel/facturas.xlsx
@@ -13,6 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
+    <sheet name="30" sheetId="2" r:id="rId5"/>
+    <sheet name="04" sheetId="3" r:id="rId6"/>
+    <sheet name="03" sheetId="4" r:id="rId7"/>
+    <sheet name="01" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +28,191 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <si>
+    <t xml:space="preserve">UUID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FECHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUBTOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONEDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIPO DE COMPROBANTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METODO DE PAGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORMA DE PAGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMISOR: RFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMISOR: NOMBRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMISOR: REGIMEN FISCAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECEPTOR: RFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECEPTOR: NOMBRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECEPTOR: USO CFDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4A7E7748-736B-4032-BEAB-325C9A34D6C6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-04T14:36:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">171586.85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">158876.71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TVN7407019H3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TUBERIAS Y VALVULAS DEL NOROESTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEI1804262B4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLIMATIZACION Y MANTENIMIENTO INDUSTRIAL RULES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3e382e73-74cd-4ccf-ac0a-f2427793b34a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-02T21:55:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1193.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1032.83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIV950315AR9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVICIOS INTERNACIONALES VICAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0004D841-2F48-46F2-8A7E-156589784D3F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-02T15:44:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2327.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2006.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLU080610C81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETN TURISTAR LUJO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4AA74EE5-DF1B-4F15-9920-2C34288F56FC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-05T12:25:38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20579.64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19055.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00bb80b5-7f86-4f49-a103-2853cfd74c0a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-08T07:49:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">874.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">753.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAN240913JR2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTOBUSES ABC DEL NOROESTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D588444-7705-4A95-B283-1E1CA673D729</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-05T13:59:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">105.84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBD180629J67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUP BC. 2018</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,4 +537,476 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
v0.0.1 Primer proyecto terminado
</commit_message>
<xml_diff>
--- a/public/excel/facturas.xlsx
+++ b/public/excel/facturas.xlsx
@@ -13,10 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
-    <sheet name="30" sheetId="2" r:id="rId5"/>
-    <sheet name="04" sheetId="3" r:id="rId6"/>
-    <sheet name="03" sheetId="4" r:id="rId7"/>
-    <sheet name="01" sheetId="5" r:id="rId8"/>
+    <sheet name="04" sheetId="2" r:id="rId5"/>
+    <sheet name="01" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -72,106 +70,88 @@
     <t xml:space="preserve">RECEPTOR: USO CFDI</t>
   </si>
   <si>
-    <t xml:space="preserve">4A7E7748-736B-4032-BEAB-325C9A34D6C6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-04-04T14:36:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">171586.85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">158876.71</t>
+    <t xml:space="preserve">0004D841-2F48-46F2-8A7E-156589784D3F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-02T15:44:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2327.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2006.47</t>
   </si>
   <si>
     <t xml:space="preserve">MXN</t>
   </si>
   <si>
-    <t xml:space="preserve">E</t>
+    <t xml:space="preserve">I</t>
   </si>
   <si>
     <t xml:space="preserve">PUE</t>
   </si>
   <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TVN7407019H3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TUBERIAS Y VALVULAS DEL NOROESTE</t>
+    <t xml:space="preserve">04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLU080610C81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETN TURISTAR LUJO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEI1804262B4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLIMATIZACION Y MANTENIMIENTO INDUSTRIAL RULES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3e382e73-74cd-4ccf-ac0a-f2427793b34a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-02T21:55:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1193.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1032.83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIV950315AR9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVICIOS INTERNACIONALES VICAM</t>
   </si>
   <si>
     <t xml:space="preserve">601</t>
   </si>
   <si>
-    <t xml:space="preserve">CEI1804262B4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLIMATIZACION Y MANTENIMIENTO INDUSTRIAL RULES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3e382e73-74cd-4ccf-ac0a-f2427793b34a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-04-02T21:55:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1193.55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1032.83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIV950315AR9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SERVICIOS INTERNACIONALES VICAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0004D841-2F48-46F2-8A7E-156589784D3F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-04-02T15:44:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2327.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2006.47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TLU080610C81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETN TURISTAR LUJO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">624</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4AA74EE5-DF1B-4F15-9920-2C34288F56FC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-04-05T12:25:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20579.64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19055.22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03</t>
+    <t xml:space="preserve">2D588444-7705-4A95-B283-1E1CA673D729</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-05T13:59:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">105.84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBD180629J67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUP BC. 2018</t>
   </si>
   <si>
     <t xml:space="preserve">00bb80b5-7f86-4f49-a103-2853cfd74c0a</t>
@@ -186,31 +166,10 @@
     <t xml:space="preserve">753.44</t>
   </si>
   <si>
-    <t xml:space="preserve">01</t>
-  </si>
-  <si>
     <t xml:space="preserve">AAN240913JR2</t>
   </si>
   <si>
     <t xml:space="preserve">AUTOBUSES ABC DEL NOROESTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2D588444-7705-4A95-B283-1E1CA673D729</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-04-05T13:59:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">105.84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">98.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBD180629J67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GROUP BC. 2018</t>
   </si>
 </sst>
 </file>
@@ -631,6 +590,50 @@
         <v>27</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
@@ -685,37 +688,37 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" t="s">
         <v>34</v>
-      </c>
-      <c r="J2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
       </c>
       <c r="L2" t="s">
         <v>25</v>
@@ -729,270 +732,34 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="J3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
         <v>47</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" t="s">
-        <v>60</v>
       </c>
       <c r="K3" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
fix: updated the download button
</commit_message>
<xml_diff>
--- a/public/excel/facturas.xlsx
+++ b/public/excel/facturas.xlsx
@@ -705,6 +705,94 @@
         <v>27</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>